<commit_message>
Update Lin Regression Example.xlsx
</commit_message>
<xml_diff>
--- a/2.Regression/Lin Regression Example.xlsx
+++ b/2.Regression/Lin Regression Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paragpradhan/Documents/Data Science Course/DSB7/2.Regression/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9488061-563A-CF4E-B069-D7F2AD4740B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78BB914C-59A9-4348-B6F6-F113EE7FEE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16080" xr2:uid="{B072FA15-93E3-8E4B-A4E1-080859142BDD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Sqft (100 x)</t>
   </si>
@@ -50,12 +50,21 @@
   <si>
     <t>(XT X)^-1</t>
   </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -63,8 +72,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -89,6 +105,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -102,11 +124,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,19 +446,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{409EA0B7-A7FC-7747-B1B8-4E5F2ACA43D3}">
-  <dimension ref="A2:K23"/>
+  <dimension ref="A2:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
       <c r="J2" s="1">
         <v>1</v>
       </c>
@@ -441,11 +472,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J3" s="1">
@@ -455,11 +486,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
         <v>10</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="6">
         <v>9</v>
       </c>
       <c r="J4" s="1">
@@ -469,11 +500,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
         <v>15</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="6">
         <v>12</v>
       </c>
       <c r="D5" t="s">
@@ -501,11 +532,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
         <v>17</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="6">
         <v>14</v>
       </c>
       <c r="E6" s="2">
@@ -530,19 +561,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <v>8</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="6">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>14</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="6">
         <v>12</v>
       </c>
       <c r="D8" t="s">
@@ -600,7 +631,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:13" x14ac:dyDescent="0.2">
       <c r="E17" s="2">
         <v>9</v>
       </c>
@@ -620,12 +651,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:13" x14ac:dyDescent="0.2">
       <c r="J18">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D20" s="3" t="s">
         <v>3</v>
       </c>
@@ -633,14 +664,70 @@
         <f>J14*E16+J15*F16+J16*G16+H16*J17+I16*J18</f>
         <v>64</v>
       </c>
-      <c r="F20" s="3">
+    </row>
+    <row r="21" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="E21" s="3">
         <f>J14*E17+J15*F17+J16*G17+H17*J17+I17*J18</f>
         <v>724</v>
       </c>
     </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
         <v>4</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" s="4">
+        <v>601</v>
+      </c>
+      <c r="G23" s="4">
+        <v>-53</v>
+      </c>
+      <c r="I23">
+        <f>$F$23*E25</f>
+        <v>3.0663265306122445</v>
+      </c>
+      <c r="J23">
+        <f>$G$23*E25</f>
+        <v>-0.27040816326530609</v>
+      </c>
+      <c r="L23" t="s">
+        <v>7</v>
+      </c>
+      <c r="M23">
+        <f>F23*E20 + G23*E21</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <f>E8*F9 - F8*E9</f>
+        <v>196</v>
+      </c>
+      <c r="F24" s="4">
+        <v>-53</v>
+      </c>
+      <c r="G24" s="4">
+        <v>5</v>
+      </c>
+      <c r="I24">
+        <f>$F$24*E25</f>
+        <v>-0.27040816326530609</v>
+      </c>
+      <c r="J24">
+        <f>$G$24*E25</f>
+        <v>2.551020408163265E-2</v>
+      </c>
+      <c r="M24">
+        <f>F24*E20 + G24*E21</f>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="25" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <f>E23/E24</f>
+        <v>5.1020408163265302E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>